<commit_message>
Module 9 assignment completed
</commit_message>
<xml_diff>
--- a/unit-3/D3/d3-coordinated-viz/data/Incarceration Rates by Country.xlsx
+++ b/unit-3/D3/d3-coordinated-viz/data/Incarceration Rates by Country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronjing/Desktop/webdir/19_g575/unit-3/D3/d3-coordinated-viz/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAF2D1B-4988-4A4B-8C79-E20ACAEBDD1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE929E4-6DE2-8842-A549-2F9A30337700}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="480" windowWidth="25040" windowHeight="15120" xr2:uid="{D1B77ECB-6D08-6041-9438-5138E1A39EFF}"/>
+    <workbookView xWindow="6020" yWindow="460" windowWidth="25040" windowHeight="15120" xr2:uid="{D1B77ECB-6D08-6041-9438-5138E1A39EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,86 +555,86 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="2">
-        <v>1548498</v>
+        <v>874161</v>
       </c>
       <c r="E3" s="1">
-        <v>118</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>615</v>
+      </c>
+      <c r="F3" s="1">
+        <v>79.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>16.899999999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>4.5999999999999996</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2">
-        <v>874161</v>
+        <v>162602</v>
       </c>
       <c r="E4" s="1">
-        <v>615</v>
+        <v>350</v>
       </c>
       <c r="F4" s="1">
-        <v>79.5</v>
+        <v>101.3</v>
       </c>
       <c r="G4" s="1">
-        <v>16.899999999999999</v>
+        <v>19.5</v>
       </c>
       <c r="H4" s="1">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2">
-        <v>371482</v>
+        <v>158501</v>
       </c>
       <c r="E5" s="1">
-        <v>193</v>
+        <v>334</v>
       </c>
       <c r="F5" s="1">
-        <v>150.9</v>
+        <v>138.6</v>
       </c>
       <c r="G5" s="1">
-        <v>33.1</v>
+        <v>27.5</v>
       </c>
       <c r="H5" s="1">
-        <v>5.4</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2">
-        <v>332112</v>
+        <v>89546</v>
       </c>
       <c r="E6" s="1">
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="F6" s="1">
-        <v>139</v>
+        <v>124.4</v>
       </c>
       <c r="G6" s="1">
-        <v>70.099999999999994</v>
+        <v>16.8</v>
       </c>
       <c r="H6" s="1">
-        <v>3.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -660,191 +660,191 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2">
-        <v>162602</v>
+        <v>371482</v>
       </c>
       <c r="E8" s="1">
-        <v>350</v>
+        <v>193</v>
       </c>
       <c r="F8" s="1">
-        <v>101.3</v>
+        <v>150.9</v>
       </c>
       <c r="G8" s="1">
-        <v>19.5</v>
+        <v>33.1</v>
       </c>
       <c r="H8" s="1">
-        <v>6.1</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="2">
-        <v>158501</v>
+        <v>47036</v>
       </c>
       <c r="E9" s="1">
-        <v>334</v>
+        <v>130</v>
       </c>
       <c r="F9" s="1">
-        <v>138.6</v>
+        <v>284.3</v>
       </c>
       <c r="G9" s="1">
-        <v>27.5</v>
+        <v>45.6</v>
       </c>
       <c r="H9" s="1">
-        <v>2.1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2">
-        <v>89546</v>
+        <v>25790</v>
       </c>
       <c r="E10" s="1">
-        <v>235</v>
+        <v>125</v>
       </c>
       <c r="F10" s="1">
-        <v>124.4</v>
+        <v>105.9</v>
       </c>
       <c r="G10" s="1">
-        <v>16.8</v>
+        <v>21.6</v>
       </c>
       <c r="H10" s="1">
-        <v>3</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="2">
-        <v>79052</v>
+        <v>1548498</v>
       </c>
       <c r="E11" s="1">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1">
-        <v>105.9</v>
-      </c>
-      <c r="G11" s="1">
-        <v>14.7</v>
+        <v>118</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H11" s="1">
-        <v>5.9</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2">
-        <v>47036</v>
+        <v>65458</v>
       </c>
       <c r="E12" s="1">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="F12" s="1">
-        <v>284.3</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="G12" s="1">
-        <v>45.6</v>
+        <v>47.7</v>
       </c>
       <c r="H12" s="1">
-        <v>42</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2">
-        <v>65458</v>
+        <v>3048</v>
       </c>
       <c r="E13" s="1">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1">
-        <v>77.400000000000006</v>
+        <v>92.1</v>
       </c>
       <c r="G13" s="1">
-        <v>47.7</v>
+        <v>15.9</v>
       </c>
       <c r="H13" s="1">
-        <v>3.3</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2">
-        <v>40444</v>
+        <v>79052</v>
       </c>
       <c r="E14" s="1">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1">
-        <v>101.5</v>
+        <v>105.9</v>
       </c>
       <c r="G14" s="1">
-        <v>64.3</v>
+        <v>14.7</v>
       </c>
       <c r="H14" s="1">
-        <v>1.9</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2">
-        <v>25790</v>
+        <v>332112</v>
       </c>
       <c r="E15" s="1">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1">
-        <v>105.9</v>
+        <v>139</v>
       </c>
       <c r="G15" s="1">
-        <v>21.6</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="H15" s="1">
-        <v>7.1</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="2">
-        <v>3048</v>
+        <v>40444</v>
       </c>
       <c r="E16" s="1">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1">
-        <v>92.1</v>
+        <v>101.5</v>
       </c>
       <c r="G16" s="1">
-        <v>15.9</v>
+        <v>64.3</v>
       </c>
       <c r="H16" s="1">
-        <v>4.8</v>
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>